<commit_message>
Added Excel File for Character and Building #2
</commit_message>
<xml_diff>
--- a/data/Cards.xlsx
+++ b/data/Cards.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unice-my.sharepoint.com/personal/matis_herrmann_etu_unice_fr/Documents/Cours/S5/PS5/Citadelles/projet2-ps5-21-22-ps5-21-22-projet2-h/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69DB1853-2FA7-4D97-BBEA-3263D4D643F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{69DB1853-2FA7-4D97-BBEA-3263D4D643F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F8D6540-0631-40D5-8A02-41FD6F65191E}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="240" windowWidth="13815" windowHeight="15105"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>Id</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Effects</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
   </si>
   <si>
     <t>Université</t>
-  </si>
-  <si>
-    <t>Points = Price + 2</t>
   </si>
   <si>
     <t xml:space="preserve">	Cette réalisation de prestige (nul n'a jamais compris à quoi pouvait bien servir une université) coûte six pièces d'or à bâtir mais vaux huit points dans le décompte de fin de partie.</t>
@@ -178,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1012,21 +1006,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="206.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="206.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,629 +1038,545 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12">
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13">
         <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14">
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19">
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>32</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21">
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>38</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23">
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>40</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25">
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26">
         <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>46</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27">
         <v>6</v>
       </c>
       <c r="F27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>47</v>
-      </c>
-      <c r="G27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E28">
         <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data from excels to instantiated Objects that is stored in a Class called Deck #2
</commit_message>
<xml_diff>
--- a/data/Cards.xlsx
+++ b/data/Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unice-my.sharepoint.com/personal/matis_herrmann_etu_unice_fr/Documents/Cours/S5/PS5/Citadelles/projet2-ps5-21-22-ps5-21-22-projet2-h/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{69DB1853-2FA7-4D97-BBEA-3263D4D643F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F8D6540-0631-40D5-8A02-41FD6F65191E}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{69DB1853-2FA7-4D97-BBEA-3263D4D643F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F965EEEB-C000-45B3-8102-E1F4FD6E9525}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>Religion</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>Église</t>
   </si>
   <si>
@@ -160,13 +157,16 @@
     <t>Université</t>
   </si>
   <si>
-    <t xml:space="preserve">	Cette réalisation de prestige (nul n'a jamais compris à quoi pouvait bien servir une université) coûte six pièces d'or à bâtir mais vaux huit points dans le décompte de fin de partie.</t>
-  </si>
-  <si>
     <t>Dracoport</t>
   </si>
   <si>
-    <t xml:space="preserve">	Cette réalisation de prestige (on n'a pas vu de dragon dans le Royaume depuis bientôt mille ans) coûte six pièces d'or à bâtir mais vaut huit points dans le décompte de fin de partie.</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Cette réalisation de prestige (nul n'a jamais compris à quoi pouvait bien servir une université) coûte six pièces d'or à bâtir mais vaux huit points dans le décompte de fin de partie.</t>
+  </si>
+  <si>
+    <t>Cette réalisation de prestige (on n'a pas vu de dragon dans le Royaume depuis bientôt mille ans) coûte six pièces d'or à bâtir mais vaut huit points dans le décompte de fin de partie.</t>
   </si>
 </sst>
 </file>
@@ -650,8 +650,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1010,7 +1013,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,562 +1023,562 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
+      <c r="F13" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5">
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
+      <c r="F18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="1">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="F21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="1">
+        <v>5</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="1">
+        <v>5</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="1">
+        <v>5</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9">
+      <c r="F25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14">
-        <v>5</v>
-      </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15">
+      <c r="D26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="1">
+        <v>6</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="1">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17">
-        <v>3</v>
-      </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="1">
+        <v>6</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22">
-        <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23">
-        <v>5</v>
-      </c>
-      <c r="F23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25">
+      <c r="E28" s="1">
         <v>6</v>
       </c>
-      <c r="F25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26">
-        <v>6</v>
-      </c>
-      <c r="F26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27">
-        <v>6</v>
-      </c>
-      <c r="F27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28">
-        <v>6</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>